<commit_message>
Actualizo gitignore para q solo suba los archivos necesarios
</commit_message>
<xml_diff>
--- a/ciudades.xlsx
+++ b/ciudades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\CC\api-astrocc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AA34D9-99B3-4D28-9235-298A78E020E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334A7677-E465-47E9-93E6-12574DB68A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{95916D23-ED3A-4AB4-A9DE-BD81F3551D3D}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
   <si>
     <t>pais</t>
   </si>
@@ -50,6 +50,9 @@
     <t>lon</t>
   </si>
   <si>
+    <t>alicante</t>
+  </si>
+  <si>
     <t>comunidad valenciana</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
     <t>andorra la vella</t>
   </si>
   <si>
+    <t>barrio norte</t>
+  </si>
+  <si>
     <t>buenos aires</t>
   </si>
   <si>
@@ -77,6 +83,12 @@
     <t>capital federal</t>
   </si>
   <si>
+    <t>cipolletti</t>
+  </si>
+  <si>
+    <t>río negro</t>
+  </si>
+  <si>
     <t>ciudad de méxico</t>
   </si>
   <si>
@@ -95,15 +107,60 @@
     <t>coronel moldes</t>
   </si>
   <si>
+    <t>curuzú cuatiá</t>
+  </si>
+  <si>
+    <t>corrientes</t>
+  </si>
+  <si>
+    <t>ensenada</t>
+  </si>
+  <si>
+    <t>florencia</t>
+  </si>
+  <si>
+    <t>caqueta</t>
+  </si>
+  <si>
+    <t>colombia</t>
+  </si>
+  <si>
     <t>granada</t>
   </si>
   <si>
     <t>andalucía</t>
   </si>
   <si>
+    <t>guadalajara</t>
+  </si>
+  <si>
+    <t>jalisco</t>
+  </si>
+  <si>
+    <t>jesus maria</t>
+  </si>
+  <si>
     <t>la plata</t>
   </si>
   <si>
+    <t>lisboa</t>
+  </si>
+  <si>
+    <t>portugal</t>
+  </si>
+  <si>
+    <t>lomas de zamora</t>
+  </si>
+  <si>
+    <t>lund</t>
+  </si>
+  <si>
+    <t>escania</t>
+  </si>
+  <si>
+    <t>suecia</t>
+  </si>
+  <si>
     <t>málaga</t>
   </si>
   <si>
@@ -113,6 +170,12 @@
     <t>maternidad sardá</t>
   </si>
   <si>
+    <t>medellín</t>
+  </si>
+  <si>
+    <t>antioquia</t>
+  </si>
+  <si>
     <t>mendoza</t>
   </si>
   <si>
@@ -125,15 +188,24 @@
     <t>santa fe</t>
   </si>
   <si>
+    <t>monte grande</t>
+  </si>
+  <si>
     <t>montevideo</t>
   </si>
   <si>
     <t>uruguay</t>
   </si>
   <si>
+    <t>moreno</t>
+  </si>
+  <si>
     <t>munro</t>
   </si>
   <si>
+    <t>neuquén</t>
+  </si>
+  <si>
     <t>palermo</t>
   </si>
   <si>
@@ -152,12 +224,18 @@
     <t>rafaela</t>
   </si>
   <si>
-    <t>río cuarto</t>
-  </si>
-  <si>
     <t>rosario</t>
   </si>
   <si>
+    <t>san fernando</t>
+  </si>
+  <si>
+    <t>san miguel</t>
+  </si>
+  <si>
+    <t>san rafael</t>
+  </si>
+  <si>
     <t>sarmiento</t>
   </si>
   <si>
@@ -173,6 +251,12 @@
     <t>chile</t>
   </si>
   <si>
+    <t>tierra del fuego</t>
+  </si>
+  <si>
+    <t>usuahia</t>
+  </si>
+  <si>
     <t>tostado</t>
   </si>
   <si>
@@ -189,6 +273,81 @@
   </si>
   <si>
     <t>lat</t>
+  </si>
+  <si>
+    <t>avellaneda</t>
+  </si>
+  <si>
+    <t>barquisimento</t>
+  </si>
+  <si>
+    <t>lara</t>
+  </si>
+  <si>
+    <t>venezuela</t>
+  </si>
+  <si>
+    <t>bogotá</t>
+  </si>
+  <si>
+    <t>cundinamarca</t>
+  </si>
+  <si>
+    <t>calafate</t>
+  </si>
+  <si>
+    <t>santa cruz</t>
+  </si>
+  <si>
+    <t>caracas</t>
+  </si>
+  <si>
+    <t>distrito capital</t>
+  </si>
+  <si>
+    <t>cumbrecita</t>
+  </si>
+  <si>
+    <t>embarcacion</t>
+  </si>
+  <si>
+    <t>humberto primo</t>
+  </si>
+  <si>
+    <t>monte buey</t>
+  </si>
+  <si>
+    <t>cordoba</t>
+  </si>
+  <si>
+    <t>pasaje pujoi</t>
+  </si>
+  <si>
+    <t>perito moreno</t>
+  </si>
+  <si>
+    <t>posadas</t>
+  </si>
+  <si>
+    <t>misiones</t>
+  </si>
+  <si>
+    <t>rio cuarto</t>
+  </si>
+  <si>
+    <t>san miguel de tucumán</t>
+  </si>
+  <si>
+    <t>tucumán</t>
+  </si>
+  <si>
+    <t>sunchales</t>
+  </si>
+  <si>
+    <t>valladoi</t>
+  </si>
+  <si>
+    <t>castilla</t>
   </si>
 </sst>
 </file>
@@ -258,6 +417,7 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="DATOS ENERGETICOS CC"/>
+      <sheetName val="Hoja2"/>
       <sheetName val="matriz144"/>
       <sheetName val="Bases"/>
       <sheetName val="Hoja1"/>
@@ -273,6 +433,7 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -595,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F90142-1127-47EE-8BE9-B0E9B3D4CB50}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,16 +770,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -626,350 +787,732 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C160">
-    <sortCondition ref="A2:A160"/>
-  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A161 A2:A32" xr:uid="{73CD30C3-3BFD-422A-A2FE-21A9206F912A}">
       <formula1>list_ciudades</formula1>

</xml_diff>